<commit_message>
Fix excel report bugs
</commit_message>
<xml_diff>
--- a/report_template/calibration_daily.xlsx
+++ b/report_template/calibration_daily.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\webApp\AQM\report_template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\webApp\TSMC_AQMS\report_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11505"/>
   </bookViews>
   <sheets>
     <sheet name="校正日報表" sheetId="1" r:id="rId1"/>
@@ -24,9 +24,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>校正日報表</t>
-  </si>
-  <si>
-    <t>測站名稱：麥寮環境監測中心</t>
   </si>
   <si>
     <t>測站名稱</t>
@@ -86,6 +83,10 @@
   </si>
   <si>
     <t>標示說明:</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>測站名稱：台積電監測車</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -247,18 +248,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="176" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -275,6 +264,18 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -379,6 +380,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -414,6 +432,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -593,7 +628,7 @@
   <dimension ref="A1:M200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A3" sqref="A3:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -607,99 +642,99 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="21"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
+    </row>
+    <row r="4" spans="1:13" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="7" t="s">
-        <v>17</v>
+      <c r="B4" s="11" t="s">
+        <v>2</v>
       </c>
-      <c r="J3" s="8" t="s">
-        <v>12</v>
+      <c r="C4" s="11" t="s">
+        <v>3</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="D4" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
-    </row>
-    <row r="4" spans="1:13" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="12" t="s">
+      <c r="G4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="H4" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="I4" s="12" t="s">
+      <c r="L4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="K4" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="L4" s="11" t="s">
+      <c r="M4" s="11" t="s">
         <v>10</v>
-      </c>
-      <c r="M4" s="11" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -3667,21 +3702,21 @@
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="17"/>
-      <c r="B1" s="18" t="s">
+      <c r="A1" s="13"/>
+      <c r="B1" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="19" t="s">
-        <v>13</v>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="16"/>
+      <c r="B2" s="17" t="s">
+        <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="20"/>
-      <c r="B2" s="21" t="s">
+      <c r="C2" s="18" t="s">
         <v>12</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>